<commit_message>
Updated with LDA and dependency parsing
</commit_message>
<xml_diff>
--- a/backend/clusters.xlsx
+++ b/backend/clusters.xlsx
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>From which state are you?</t>
+          <t>What is your age?</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -461,14 +461,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>From which state are you?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Why are you...?</t>
+          <t>From which state are you?</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -476,592 +476,592 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>From which state are you?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Why is the value for j taken as 2?</t>
+          <t>Why use insertion sort when you can use more efficient algorithms like quick sort?</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Why is the value for j taken as 2?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Why is there j=2 in the for loop?</t>
+          <t>Is that index which is written above array?</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Why is the value for j taken as 2?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Why is the value of j taken as 2 in the for loop?</t>
+          <t>Why was the array index starting from 1?</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Why is the value for j taken as 2?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>I was confused between j and key while explaining.</t>
+          <t>Is insertion sort the best among all sorting algorithms, or if not, why is it slower than others?</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Why is the value for j taken as 2?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Why did we start from j=2 instead of j=1?</t>
+          <t>Is that the index on the box 1,2,3,4,5,6,7,8,9? If yes, then it should start from 0.</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Why is the value for j taken as 2?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Is that index which is written above array?</t>
+          <t>Is it okay to learn the same experiment from other sources?</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Why was the array index starting from 1?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Why was the array index starting from 1?</t>
+          <t>How does the insertion sort algorithm handle duplicate elements?</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Why was the array index starting from 1?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Why did the array indexing start from 1 rather than 0?</t>
+          <t>Which algorithm makes switching of two arrays possible?</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Why was the array index starting from 1?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Is that the index on the box 1,2,3,4,5,6,7,8,9? If yes, then it should start from 0.</t>
+          <t>Why are you...?</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Why was the array index starting from 1?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>The array index starts from 0, but here you have taken 1. Why?</t>
+          <t>Why use insertion sort when there are more efficient algorithms like quick sort?</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Why was the array index starting from 1?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>How to calculate the space complexity (explain in detail).</t>
+          <t>The array index starts from 0, but here you have taken 1. Why?</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>How to calculate the space complexity (explain in detail).</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>How to determine space complexity?</t>
+          <t>For considering the number of comparisons, we take value 1, but the while condition has &amp;&amp; in it, so two comparisons will be made: i&gt;0 and A[i] &gt; key. Then why is the value 1?</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>How to calculate the space complexity (explain in detail).</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>I did not understand how to calculate space complexity.</t>
+          <t>How does the algorithm compare each element to the others?</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>How to calculate the space complexity (explain in detail).</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>How is space complexity calculated for different cases?</t>
+          <t>What is the purpose of the key element in insertion sort?</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>How to calculate the space complexity (explain in detail).</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>How to calculate space complexity for complex code?</t>
+          <t>Insertion sort algorithm makes many operations even for an already sorted ascending list. What is the advantage of using it?</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>How to calculate the space complexity (explain in detail).</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>I did not understand space complexity.</t>
+          <t>While calculating time complexity, if the array is neither in ascending nor descending order, the number of operations for each value of j can differ. So why have we generalized it to (n-1)?</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>How to calculate the space complexity (explain in detail).</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>How to calculate space complexity?</t>
+          <t>Insertion sort seems like a time-consuming option compared to other sorting techniques. Where/why would we use such a non-feasible method?</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>How to calculate the space complexity (explain in detail).</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>How is space complexity calculated for different cases?</t>
+          <t>How is the insertion sort algorithm different from bubble sort and selection sort?</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>How to calculate the space complexity (explain in detail).</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Could you explain the space complexity concept?</t>
+          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>How to calculate the space complexity (explain in detail).</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>How was time complexity determined?</t>
+          <t>I was confused between j and key while explaining.</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>How is time complexity calculated?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>What is complexity, and how to calculate complexity?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>How is time complexity calculated?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>What is the formula for complexity?</t>
+          <t>What is the difference between insertion sort and bubble sort?</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>How is time complexity calculated?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>How to determine time complexity?</t>
+          <t>What if all elements of an array are the same?</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>How is time complexity calculated?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>How is time complexity calculated?</t>
+          <t>Where do we use insertion sort in real-life applications?</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>How is time complexity calculated?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>How to calculate time complexity?</t>
+          <t>Does space complexity change if the number of elements in an array varies?</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>How is time complexity calculated?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>What are the efficient ways to calculate time and space complexity according to an algorithm or code?</t>
+          <t>If an element at index i is already at its correct position, can there still be out-of-order elements before it?</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>How is time complexity calculated?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Between insertion sort and bubble sort, which is more reliable?</t>
+          <t>Do we require extra memory for merge sort?</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>What is the difference between insertion sort and bubble sort?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>How is the insertion sort algorithm different from bubble sort and selection sort?</t>
+          <t>In which scenario should we use insertion sort?</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>What is the difference between insertion sort and bubble sort?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>How does insertion sort differ from selection sort or bubble sort?</t>
+          <t>What is the difference between merge sort and insertion sort?</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>What is the difference between insertion sort and bubble sort?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>What is the difference between insertion sort and bubble sort?</t>
+          <t>Is this algorithm generalized for all cases?</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>What is the difference between insertion sort and bubble sort?</t>
+          <t>How does insertion sort differ from selection sort or bubble sort?</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Why use insertion sort when you can use more efficient algorithms like quick sort?</t>
+          <t>Between insertion sort and bubble sort, which is more reliable?</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Is insertion sort the best among all sorting algorithms, or if not, why is it slower than others?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Is insertion sort the most optimal sorting algorithm among all sorting algorithms?</t>
+          <t>If the data quantity is large, is insertion sort the best option? If not, why?</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Is insertion sort the best among all sorting algorithms, or if not, why is it slower than others?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Is insertion sort the best among all sorting algorithms, or if not, why is it slower than others?</t>
+          <t>How was time complexity determined?</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Is insertion sort the best among all sorting algorithms, or if not, why is it slower than others?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Is insertion sort the most optimal sorting algorithm among all sorting algorithms?</t>
+          <t>Can you explain ascending order and descending order best and worst case scenarios again?</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Is insertion sort the best among all sorting algorithms, or if not, why is it slower than others?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Why use insertion sort when there are more efficient algorithms like quick sort?</t>
+          <t>Is insertion sort suitable for data?</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Is insertion sort the best among all sorting algorithms, or if not, why is it slower than others?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Why is insertion sort considered more efficient for small or nearly sorted datasets?</t>
+          <t>How does the worst case happen in descending order?</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Is insertion sort the best among all sorting algorithms, or if not, why is it slower than others?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>If the data quantity is large, is insertion sort the best option? If not, why?</t>
+          <t>On what basis are best, worst, and average cases determined? Can we start comparison from j=1 to the total length of the array?</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>If the data quantity is large, is insertion sort the best option? If not, why?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Is insertion sort suitable for data?</t>
+          <t>I didn't understand how to calculate the space complexity for the worst-case scenario in insertion sort.</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>If the data quantity is large, is insertion sort the best option? If not, why?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>For which dataset size is insertion sort more suitable?</t>
+          <t>In insertion sort, how do we know if this is the best condition or worst? If the number is not in ascending or descending order?</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>If the data quantity is large, is insertion sort the best option? If not, why?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
@@ -1072,26 +1072,26 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Where and why is insertion sort used?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>What are the space complexities of insertion sort in different ways?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Where and why is insertion sort used?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
@@ -1102,1181 +1102,1181 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Where and why is insertion sort used?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>What is insertion sort?</t>
+          <t>What is the time complexity of insertion sort in the best, worst, and average cases?</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Where and why is insertion sort used?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Can you give a real-world application example of insertion sort?</t>
+          <t>Could insertion sort be modified to work in descending order?</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Where and why is insertion sort used?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Where do we use insertion sort in real-life applications?</t>
+          <t>For the best case, if we insert the array in ascending order, what are the perks of using insertion sort when it is already sorted?</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Where and why is insertion sort used?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>What is the time complexity of insertion sort in the best, worst, and average cases?</t>
+          <t>I am not able to code insertion sort on my own. What could help me with that?</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>What is the time complexity of insertion sort in the best, worst, and average cases?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>What are the time complexities of insertion sort in best, average, and worst cases?</t>
+          <t>What is the average-case time complexity for this algorithm?</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>What is the time complexity of insertion sort in the best, worst, and average cases?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>What is the worst-case time complexity of insertion sort, and why does it occur?</t>
+          <t>What is insertion sort?</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>What is the time complexity of insertion sort in the best, worst, and average cases?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>What is space complexity in the insertion sort algorithm?</t>
+          <t>What is the average case scenario for this array?</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>What is space complexity in the insertion sort algorithm?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>What is space complexity in insertion sorting?</t>
+          <t>Does insertion sort work effectively on large arrays?</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>What is space complexity in the insertion sort algorithm?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>How to find the space complexity for insertion sort?</t>
+          <t>Can you give a real-world application example of insertion sort?</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>What is space complexity in the insertion sort algorithm?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>I didn't understand how to calculate the space complexity for the worst-case scenario in insertion sort.</t>
+          <t>What will happen if we pass an empty array?</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>What is space complexity in the insertion sort algorithm?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>What is your age?</t>
+          <t>How does insertion sort perform on a reverse-sorted array?</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Explain again.</t>
+          <t>What are the time complexities of insertion sort in best, average, and worst cases?</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>How did n^2 come?</t>
+          <t>For which dataset size is insertion sort more suitable?</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Doubt on time complexity equation.</t>
+          <t>What is the stability of insertion sort for handling large datasets?</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>What are other types of space complexity other than in-place?</t>
+          <t>Descending order gives O(n²) time complexity, and ascending order gives O(n). What about the average case?</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Why do we need space complexity?</t>
+          <t>What is the worst-case time complexity of insertion sort, and why does it occur?</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Why is it considered to be n² always?</t>
+          <t>What can be done to improve the worst case for insertion sort?</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>What are ways to represent them, and on what factors are they dependent?</t>
+          <t>For the best case input, what is the running time of insertion sort?</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Can insertion sort be used for linked lists as well as arrays?</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>In insertion sorting, how many sorts can be done at a time?</t>
+          <t>Explain again.</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Is it okay to learn the same experiment from other sources?</t>
+          <t>Doubt on time complexity equation.</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Can you explain ascending order and descending order best and worst case scenarios again?</t>
+          <t>What are other types of space complexity other than in-place?</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>How does the insertion sort algorithm handle duplicate elements?</t>
+          <t>What is space complexity in the insertion sort algorithm?</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Which algorithm makes switching of two arrays possible?</t>
+          <t>Is insertion sort the most optimal sorting algorithm among all sorting algorithms?</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>What will the algorithm do if there are multiple equal numbers in the list?</t>
+          <t>Why do we need space complexity?</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>If there is a program that continuously adds numbers and sorts them, is the insertion algorithm the most reliable?</t>
+          <t>How to calculate the space complexity (explain in detail).</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>How does the worst case happen in descending order?</t>
+          <t>Why is it considered to be n² always?</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Isn't it allowed for an institute to provide external study material?</t>
+          <t>How to determine space complexity?</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>On what basis are best, worst, and average cases determined? Can we start comparison from j=1 to the total length of the array?</t>
+          <t>What is space complexity in insertion sorting?</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>I don't understand the time complexity concept very well.</t>
+          <t>Is insertion sort the most optimal sorting algorithm among all sorting algorithms?</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>When discussing time complexity, I did not understand the difference between the count of comparison and swapping.</t>
+          <t>In insertion sorting, how many sorts can be done at a time?</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>For considering the number of comparisons, we take value 1, but the while condition has &amp;&amp; in it, so two comparisons will be made: i&gt;0 and A[i] &gt; key. Then why is the value 1?</t>
+          <t>What is complexity, and how to calculate complexity?</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>In insertion sort, how do we know if this is the best condition or worst? If the number is not in ascending or descending order?</t>
+          <t>What is the formula for complexity?</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>In any programming language questions, I can't understand how to approach a problem to solve it on my own.</t>
+          <t>How to determine time complexity?</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>How does the algorithm compare each element to the others?</t>
+          <t>How to find the space complexity for insertion sort?</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Can insertion sort be used for linked lists as well as arrays?</t>
+          <t>I don't understand the time complexity concept very well.</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>What is the purpose of the key element in insertion sort?</t>
+          <t>I did not understand how to calculate space complexity.</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Could insertion sort be modified to work in descending order?</t>
+          <t>How is space complexity calculated for different cases?</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>How can I choose a particular programming language to create a simple project for my resume?</t>
+          <t>How to calculate space complexity for complex code?</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Insertion sort algorithm makes many operations even for an already sorted ascending list. What is the advantage of using it?</t>
+          <t>How is time complexity calculated?</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>While calculating time complexity, if the array is neither in ascending nor descending order, the number of operations for each value of j can differ. So why have we generalized it to (n-1)?</t>
+          <t>How to calculate time complexity?</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>For the best case, if we insert the array in ascending order, what are the perks of using insertion sort when it is already sorted?</t>
+          <t>Why is the time complexity O(n²)?</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>I am not able to code insertion sort on my own. What could help me with that?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Insertion sort seems like a time-consuming option compared to other sorting techniques. Where/why would we use such a non-feasible method?</t>
+          <t>Why is space complexity O(1)?</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Why is the time complexity O(n²)?</t>
+          <t>What is the difference between time and space complexity?</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
+          <t>How to calculate space complexity?</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Why is space complexity O(1)?</t>
+          <t>How is space complexity calculated for different cases?</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>How are questions related to complexities asked in exams?</t>
+          <t>What if duplicate values appear in sorting, and how will it affect time complexity?</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>What is the difference between time and space complexity?</t>
+          <t>Why are space complexity and time complexity required in algorithm analysis?</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>What if duplicate values appear in sorting, and how will it affect time complexity?</t>
+          <t>What will be the space complexity if the user enters the array?</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>What is the average-case time complexity for this algorithm?</t>
+          <t>What are the efficient ways to calculate time and space complexity according to an algorithm or code?</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>What is the average case scenario for this array?</t>
+          <t>Why is insertion sort considered more efficient for small or nearly sorted datasets?</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Why are space complexity and time complexity required in algorithm analysis?</t>
+          <t>I need to learn from the basics to calculate with constants.</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Does insertion sort work effectively on large arrays?</t>
+          <t>If we free variables/constants before exiting the function, what would the space complexity be?</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>I didn't understand the final calculation, such as 2n, 2n², etc.</t>
+          <t>Are there online sources to study algorithm analysis?</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Could you explain the space complexity concept?</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>What will be the space complexity if the user enters the array?</t>
+          <t>Which sorting algorithm has the lowest time complexity?</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>What will happen if we pass an empty array?</t>
+          <t>Which sorting algorithm is easiest and best to use with the least time and space complexity?</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is time complexity only based on the declarations of additional arrays needed during execution?</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>What is a different method to do this?</t>
+          <t>Why is the value for j taken as 2?</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is the value of j taken as 2 in the for loop?</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>How does insertion sort perform on a reverse-sorted array?</t>
+          <t>Why is there j=2 in the for loop?</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is the value of j taken as 2 in the for loop?</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>I need to learn from the basics to calculate with constants.</t>
+          <t>Why is the value of j taken as 2 in the for loop?</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is the value of j taken as 2 in the for loop?</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>What if all elements of an array are the same?</t>
+          <t>If there is a program that continuously adds numbers and sorts them, is the insertion algorithm the most reliable?</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is the value of j taken as 2 in the for loop?</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>What is the stability of insertion sort for handling large datasets?</t>
+          <t>Isn't it allowed for an institute to provide external study material?</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is the value of j taken as 2 in the for loop?</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>If we free variables/constants before exiting the function, what would the space complexity be?</t>
+          <t>How to determine the order?</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>Why is the value of j taken as 2 in the for loop?</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Does space complexity change if the number of elements in an array varies?</t>
+          <t>How did n^2 come?</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Are there online sources to study algorithm analysis?</t>
+          <t>Why did the array indexing start from 1 rather than 0?</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>If an element at index i is already at its correct position, can there still be out-of-order elements before it?</t>
+          <t>What are ways to represent them, and on what factors are they dependent?</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Descending order gives O(n²) time complexity, and ascending order gives O(n). What about the average case?</t>
+          <t>What will the algorithm do if there are multiple equal numbers in the list?</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Do we require extra memory for merge sort?</t>
+          <t>When discussing time complexity, I did not understand the difference between the count of comparison and swapping.</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>In which scenario should we use insertion sort?</t>
+          <t>In any programming language questions, I can't understand how to approach a problem to solve it on my own.</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>What is the difference between merge sort and insertion sort?</t>
+          <t>What are the space complexities of insertion sort in different ways?</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>What can be done to improve the worst case for insertion sort?</t>
+          <t>How can I choose a particular programming language to create a simple project for my resume?</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Why do we need different sorting techniques?</t>
+          <t>I did not understand space complexity.</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Is this algorithm generalized for all cases?</t>
+          <t>How are questions related to complexities asked in exams?</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>How to determine the order?</t>
+          <t>I didn't understand the final calculation, such as 2n, 2n², etc.</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>For the best case input, what is the running time of insertion sort?</t>
+          <t>Why did we start from j=2 instead of j=1?</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
+          <t>What is a different method to do this?</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>4</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
           <t>What is the average number of inversions in an array of N distinct numbers?</t>
-        </is>
-      </c>
-      <c r="B121" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Which sorting algorithm has the lowest time complexity?</t>
+          <t>Why do we need different sorting techniques?</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Which sorting algorithm is easiest and best to use with the least time and space complexity?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>How does insertion sort handle edge cases, like if all elements in the array are identical?</t>
+          <t>What is the average number of inversions in an array of N distinct numbers?</t>
         </is>
       </c>
     </row>

</xml_diff>